<commit_message>
fix student query by klass everywhere
</commit_message>
<xml_diff>
--- a/client/public/תלמידות דוגמא.xlsx
+++ b/client/public/תלמידות דוגמא.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\SideProjects\VocalCenterStats\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEF1EB2-BD8B-4E81-A0DF-457D41364B83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB872E5F-2F39-4AEF-A240-65823638E680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22020" windowHeight="13176" xr2:uid="{FF66E609-E81F-4767-ABF8-2664ABFC9511}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>שרה כהן</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>יעל אלקריף</t>
+  </si>
+  <si>
+    <t>התמחות אנגלית</t>
+  </si>
+  <si>
+    <t>התמחות חשבון</t>
+  </si>
+  <si>
+    <t>תכנות</t>
+  </si>
+  <si>
+    <t>התעמלות</t>
   </si>
 </sst>
 </file>
@@ -419,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22870778-7611-4B42-8957-36649F81B377}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -432,7 +444,7 @@
     <col min="5" max="5" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>754752452</v>
       </c>
@@ -445,8 +457,11 @@
       <c r="D1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123412341</v>
       </c>
@@ -459,8 +474,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>234124312</v>
       </c>
@@ -473,8 +491,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>432423423</v>
       </c>
@@ -487,8 +508,11 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>452353265</v>
       </c>
@@ -501,8 +525,11 @@
       <c r="D5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>543454366</v>
       </c>
@@ -515,8 +542,11 @@
       <c r="D6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>676745643</v>
       </c>
@@ -529,8 +559,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>543776723</v>
       </c>
@@ -543,8 +576,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>463473456</v>
       </c>
@@ -557,8 +593,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>623451258</v>
       </c>
@@ -571,8 +610,11 @@
       <c r="D10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>564374574</v>
       </c>
@@ -585,8 +627,11 @@
       <c r="D11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>754243574</v>
       </c>
@@ -598,6 +643,9 @@
       </c>
       <c r="D12">
         <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>